<commit_message>
16.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Requisition of Tulip-2/Requisition of Tulip-2.xlsx
+++ b/July/Others/Requisition of Tulip-2/Requisition of Tulip-2.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="106">
   <si>
     <t>Model Name</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>L120</t>
-  </si>
-  <si>
-    <t>BL100</t>
   </si>
   <si>
     <t>BL75</t>
@@ -353,10 +350,16 @@
     <t>Dark_Blue=100,Black_Red=20</t>
   </si>
   <si>
-    <t>15.07.19</t>
-  </si>
-  <si>
     <t>Black/ Not_Red</t>
+  </si>
+  <si>
+    <t>D37</t>
+  </si>
+  <si>
+    <t>Black &amp; Gold</t>
+  </si>
+  <si>
+    <t>16.07.19</t>
   </si>
 </sst>
 </file>
@@ -1005,10 +1008,10 @@
   <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E87" sqref="E87"/>
+      <selection pane="bottomRight" activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1023,7 +1026,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="12.75">
       <c r="A1" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -1032,7 +1035,7 @@
     </row>
     <row r="2" spans="1:5" s="6" customFormat="1" ht="12.75">
       <c r="A2" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="35"/>
       <c r="C2" s="35"/>
@@ -1041,17 +1044,17 @@
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15">
       <c r="A3" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="27" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="6" customFormat="1" ht="12.75">
@@ -1084,12 +1087,12 @@
         <v>0</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" hidden="1">
       <c r="A6" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="9">
         <v>789.97</v>
@@ -1103,7 +1106,7 @@
     </row>
     <row r="7" spans="1:5" ht="15" hidden="1">
       <c r="A7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="9">
         <v>779.94500000000005</v>
@@ -1117,7 +1120,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" hidden="1">
       <c r="A8" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="9">
         <v>760.9</v>
@@ -1128,12 +1131,12 @@
         <v>0</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" hidden="1">
       <c r="A9" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="9">
         <v>769.92</v>
@@ -1144,12 +1147,12 @@
         <v>0</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" hidden="1">
       <c r="A10" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="9">
         <v>896.24</v>
@@ -1160,7 +1163,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
@@ -1176,12 +1179,12 @@
         <v>0</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" hidden="1">
       <c r="A12" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="9">
         <v>868.16499999999996</v>
@@ -1206,12 +1209,12 @@
         <v>0</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" hidden="1">
       <c r="A14" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="9">
         <v>858.14</v>
@@ -1222,26 +1225,28 @@
         <v>0</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="5" customFormat="1" ht="15">
       <c r="A15" s="11" t="s">
-        <v>33</v>
+        <v>103</v>
       </c>
       <c r="B15" s="9">
-        <v>985.45749999999998</v>
-      </c>
-      <c r="C15" s="8"/>
+        <v>858.14</v>
+      </c>
+      <c r="C15" s="8">
+        <v>39</v>
+      </c>
       <c r="D15" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>33467.46</v>
       </c>
       <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:5" ht="15" hidden="1">
       <c r="A16" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="9">
         <v>946.36</v>
@@ -1266,7 +1271,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" hidden="1">
@@ -1282,12 +1287,12 @@
         <v>0</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" hidden="1">
       <c r="A19" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="9">
         <v>1159.8900000000001</v>
@@ -1298,28 +1303,30 @@
         <v>0</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" hidden="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15">
       <c r="A20" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="9">
         <v>1140.845</v>
       </c>
-      <c r="C20" s="8"/>
+      <c r="C20" s="8">
+        <v>38</v>
+      </c>
       <c r="D20" s="12">
         <f>C20*B20</f>
-        <v>0</v>
+        <v>43352.11</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A21" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" s="9">
         <v>936.34</v>
@@ -1331,27 +1338,25 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" ht="15">
+    <row r="22" spans="1:5" ht="15" hidden="1">
       <c r="A22" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="9">
         <v>1014.53</v>
       </c>
-      <c r="C22" s="8">
-        <v>40</v>
-      </c>
+      <c r="C22" s="8"/>
       <c r="D22" s="10">
         <f t="shared" si="0"/>
-        <v>40581.199999999997</v>
+        <v>0</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" hidden="1">
       <c r="A23" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="9">
         <v>907.26</v>
@@ -1362,12 +1367,12 @@
         <v>0</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A24" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="9">
         <v>1159.8924999999999</v>
@@ -1378,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" hidden="1">
@@ -1397,7 +1402,7 @@
     </row>
     <row r="26" spans="1:5" ht="15" hidden="1">
       <c r="A26" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="9">
         <v>2710.76</v>
@@ -1408,12 +1413,12 @@
         <v>0</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" hidden="1">
       <c r="A27" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="9">
         <v>6397.96</v>
@@ -1427,7 +1432,7 @@
     </row>
     <row r="28" spans="1:5" ht="15" hidden="1">
       <c r="A28" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="9">
         <v>5158.8649999999998</v>
@@ -1438,12 +1443,12 @@
         <v>0</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" hidden="1">
       <c r="A29" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29" s="9">
         <v>5334.3029999999999</v>
@@ -1471,7 +1476,7 @@
     </row>
     <row r="31" spans="1:5" ht="15" hidden="1">
       <c r="A31" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="9">
         <v>5607.9849999999997</v>
@@ -1485,7 +1490,7 @@
     </row>
     <row r="32" spans="1:5" ht="15" hidden="1">
       <c r="A32" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B32" s="9">
         <v>5793.4475000000002</v>
@@ -1496,12 +1501,12 @@
         <v>0</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" hidden="1">
       <c r="A33" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="9">
         <v>7714.2375000000002</v>
@@ -1527,27 +1532,25 @@
       </c>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:5" ht="15">
+    <row r="35" spans="1:5" ht="15" hidden="1">
       <c r="A35" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" s="9">
         <v>6369.8850000000002</v>
       </c>
-      <c r="C35" s="8">
-        <v>11</v>
-      </c>
+      <c r="C35" s="8"/>
       <c r="D35" s="10">
         <f t="shared" si="0"/>
-        <v>70068.735000000001</v>
+        <v>0</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" hidden="1">
       <c r="A36" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="9">
         <v>8967.36</v>
@@ -1558,12 +1561,12 @@
         <v>0</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" hidden="1">
       <c r="A37" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B37" s="9">
         <v>8134.2849999999999</v>
@@ -1577,7 +1580,7 @@
     </row>
     <row r="38" spans="1:5" ht="15">
       <c r="A38" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="9">
         <v>1169.9175</v>
@@ -1590,7 +1593,7 @@
         <v>19888.5975</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" hidden="1">
@@ -1609,7 +1612,7 @@
     </row>
     <row r="40" spans="1:5" ht="15" hidden="1">
       <c r="A40" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B40" s="9">
         <v>1189.9675</v>
@@ -1662,12 +1665,12 @@
         <v>0</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" hidden="1">
       <c r="A44" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="9">
         <v>1072.675</v>
@@ -1679,27 +1682,25 @@
       </c>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="1:5" ht="15">
+    <row r="45" spans="1:5" ht="15" hidden="1">
       <c r="A45" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="9">
         <v>985.46</v>
       </c>
-      <c r="C45" s="8">
-        <v>91</v>
-      </c>
+      <c r="C45" s="8"/>
       <c r="D45" s="10">
         <f t="shared" si="0"/>
-        <v>89676.86</v>
+        <v>0</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" hidden="1">
       <c r="A46" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" s="9">
         <v>1014.53</v>
@@ -1713,7 +1714,7 @@
     </row>
     <row r="47" spans="1:5" ht="15" hidden="1">
       <c r="A47" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B47" s="9">
         <v>1072.675</v>
@@ -1724,7 +1725,7 @@
     </row>
     <row r="48" spans="1:5" ht="15" hidden="1">
       <c r="A48" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" s="9">
         <v>1077.6875</v>
@@ -1735,12 +1736,12 @@
         <v>0</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15" hidden="1">
       <c r="A49" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49" s="9">
         <v>1024.5550000000001</v>
@@ -1754,7 +1755,7 @@
     </row>
     <row r="50" spans="1:5" ht="15" hidden="1">
       <c r="A50" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B50" s="9">
         <v>1101.7474999999999</v>
@@ -1768,7 +1769,7 @@
     </row>
     <row r="51" spans="1:5" ht="15" hidden="1">
       <c r="A51" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" s="9">
         <v>1072.675</v>
@@ -1779,12 +1780,12 @@
         <v>0</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" hidden="1">
       <c r="A52" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B52" s="9">
         <v>1297.2349999999999</v>
@@ -1810,19 +1811,23 @@
       </c>
       <c r="E53" s="8"/>
     </row>
-    <row r="54" spans="1:5" ht="15" hidden="1">
+    <row r="54" spans="1:5" ht="15">
       <c r="A54" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" s="9">
         <v>5607.9849999999997</v>
       </c>
-      <c r="C54" s="8"/>
+      <c r="C54" s="8">
+        <v>10</v>
+      </c>
       <c r="D54" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="8"/>
+        <v>56079.85</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="15" hidden="1">
       <c r="A55" s="8" t="s">
@@ -1854,7 +1859,7 @@
     </row>
     <row r="57" spans="1:5" ht="15" hidden="1">
       <c r="A57" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B57" s="9">
         <v>4526.2875000000004</v>
@@ -1865,7 +1870,7 @@
         <v>0</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" hidden="1">
@@ -1884,25 +1889,25 @@
     </row>
     <row r="59" spans="1:5" ht="15">
       <c r="A59" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B59" s="9">
         <v>4896.21</v>
       </c>
       <c r="C59" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D59" s="10">
         <f t="shared" si="1"/>
-        <v>24481.05</v>
+        <v>34273.47</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15" hidden="1">
       <c r="A60" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B60" s="9">
         <v>5150.8450000000003</v>
@@ -1916,7 +1921,7 @@
     </row>
     <row r="61" spans="1:5" ht="15" hidden="1">
       <c r="A61" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B61" s="9">
         <v>4973.4025000000001</v>
@@ -1927,12 +1932,12 @@
         <v>0</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15" hidden="1">
       <c r="A62" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B62" s="9">
         <v>4701.7299999999996</v>
@@ -1943,12 +1948,12 @@
         <v>0</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" hidden="1">
       <c r="A63" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B63" s="9">
         <v>5940.8149999999996</v>
@@ -1962,7 +1967,7 @@
     </row>
     <row r="64" spans="1:5" ht="15" hidden="1">
       <c r="A64" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B64" s="9">
         <v>5257.11</v>
@@ -1990,7 +1995,7 @@
     </row>
     <row r="66" spans="1:5" ht="15" hidden="1">
       <c r="A66" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B66" s="9">
         <v>3471.6574999999998</v>
@@ -2001,12 +2006,12 @@
         <v>0</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15" hidden="1">
       <c r="A67" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B67" s="9">
         <v>3257.1224999999999</v>
@@ -2017,30 +2022,28 @@
         <v>0</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="15">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15" hidden="1">
       <c r="A68" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B68" s="9">
         <v>4389.9475000000002</v>
       </c>
-      <c r="C68" s="8">
-        <v>5</v>
-      </c>
+      <c r="C68" s="8"/>
       <c r="D68" s="10">
         <f t="shared" si="1"/>
-        <v>21949.737500000003</v>
+        <v>0</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15" hidden="1">
       <c r="A69" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B69" s="9">
         <v>3618.0225</v>
@@ -2051,12 +2054,12 @@
         <v>0</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15" hidden="1">
       <c r="A70" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B70" s="9">
         <v>3530.8049999999998</v>
@@ -2067,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" hidden="1">
@@ -2086,7 +2089,7 @@
     </row>
     <row r="72" spans="1:5" ht="15" hidden="1">
       <c r="A72" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B72" s="9">
         <v>4408.9949999999999</v>
@@ -2100,7 +2103,7 @@
     </row>
     <row r="73" spans="1:5" ht="15" hidden="1">
       <c r="A73" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B73" s="9">
         <v>3979.9250000000002</v>
@@ -2111,28 +2114,30 @@
         <v>0</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="15" hidden="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15">
       <c r="A74" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" s="9">
         <v>4115.2624999999998</v>
       </c>
-      <c r="C74" s="8"/>
+      <c r="C74" s="8">
+        <v>3</v>
+      </c>
       <c r="D74" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12345.787499999999</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" hidden="1">
       <c r="A75" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B75" s="9">
         <v>1219.04</v>
@@ -2143,12 +2148,12 @@
         <v>0</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15" hidden="1">
       <c r="A76" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B76" s="9">
         <v>8599.4449999999997</v>
@@ -2167,11 +2172,11 @@
       <c r="B77" s="37"/>
       <c r="C77" s="24">
         <f>SUM(C5:C76)</f>
-        <v>169</v>
+        <v>114</v>
       </c>
       <c r="D77" s="25">
         <f>SUM(D5:D76)</f>
-        <v>266646.18</v>
+        <v>199407.27500000002</v>
       </c>
       <c r="E77" s="24"/>
     </row>
@@ -2230,7 +2235,7 @@
         <v>22</v>
       </c>
       <c r="C84" s="29">
-        <v>270000</v>
+        <v>200000</v>
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="14"/>
@@ -2278,7 +2283,7 @@
       </c>
       <c r="C89" s="30">
         <f>SUM(C83:C88)</f>
-        <v>270000</v>
+        <v>200000</v>
       </c>
       <c r="D89" s="20"/>
       <c r="E89" s="14"/>

</xml_diff>

<commit_message>
18.07.19 Today Morning 12:26 PM Updated
</commit_message>
<xml_diff>
--- a/July/Others/Requisition of Tulip-2/Requisition of Tulip-2.xlsx
+++ b/July/Others/Requisition of Tulip-2/Requisition of Tulip-2.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Daily Requisition'!$A$4:$E$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Daily Requisition'!$A$4:$E$79</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="108">
   <si>
     <t>Model Name</t>
   </si>
@@ -297,9 +297,6 @@
   </si>
   <si>
     <t>L55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gold </t>
   </si>
   <si>
     <t>B12+</t>
@@ -362,7 +359,13 @@
     <t>T140</t>
   </si>
   <si>
-    <t>17.07.19</t>
+    <t>BL97</t>
+  </si>
+  <si>
+    <t>18.07.19</t>
+  </si>
+  <si>
+    <t>Gold/Black</t>
   </si>
 </sst>
 </file>
@@ -1008,13 +1011,13 @@
   <sheetPr filterMode="1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E87" sqref="E87"/>
+      <selection pane="bottomRight" activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1102,7 +1105,7 @@
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="10">
-        <f t="shared" ref="D6:D54" si="0">C6*B6</f>
+        <f t="shared" ref="D6:D55" si="0">C6*B6</f>
         <v>0</v>
       </c>
       <c r="E6" s="8"/>
@@ -1123,7 +1126,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" hidden="1">
       <c r="A8" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="9">
         <v>760.9</v>
@@ -1134,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" hidden="1">
@@ -1150,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" hidden="1">
@@ -1228,141 +1231,141 @@
         <v>0</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" ht="15">
-      <c r="A15" s="11" t="s">
-        <v>103</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15">
+      <c r="A15" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="B15" s="9">
+        <v>824.06</v>
+      </c>
+      <c r="C15" s="8">
+        <v>58</v>
+      </c>
+      <c r="D15" s="10">
+        <f>B15*C15</f>
+        <v>47795.479999999996</v>
+      </c>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+      <c r="A16" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="9">
         <v>858.14</v>
       </c>
-      <c r="C15" s="8">
-        <v>39</v>
-      </c>
-      <c r="D15" s="12">
-        <f t="shared" si="0"/>
-        <v>33467.46</v>
-      </c>
-      <c r="E15" s="11" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" hidden="1">
-      <c r="A16" s="8" t="s">
+    <row r="17" spans="1:5" ht="15" hidden="1">
+      <c r="A17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B17" s="9">
         <v>946.36</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
-      <c r="A17" s="11" t="s">
+      <c r="C17" s="8"/>
+      <c r="D17" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+      <c r="A18" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B18" s="9">
         <v>980.44500000000005</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="12">
-        <f>C17*B17</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="11" t="s">
+      <c r="C18" s="8"/>
+      <c r="D18" s="12">
+        <f>C18*B18</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" hidden="1">
-      <c r="A18" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="9">
-        <v>975.4325</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" hidden="1">
       <c r="A19" s="8" t="s">
-        <v>98</v>
+        <v>4</v>
       </c>
       <c r="B19" s="9">
-        <v>1159.8900000000001</v>
+        <v>975.4325</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="10">
-        <f>B19*C19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" hidden="1">
       <c r="A20" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="9">
+        <v>1159.8900000000001</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="10">
+        <f>B20*C20</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15">
+      <c r="A21" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B21" s="9">
         <v>1140.845</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="12">
-        <f>C20*B20</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
-      <c r="A21" s="11" t="s">
+      <c r="C21" s="8">
+        <v>38</v>
+      </c>
+      <c r="D21" s="12">
+        <f>C21*B21</f>
+        <v>43352.11</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+      <c r="A22" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B22" s="9">
         <v>936.34</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" ht="15" hidden="1">
-      <c r="A22" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="9">
-        <v>1014.53</v>
-      </c>
       <c r="C22" s="8"/>
-      <c r="D22" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="D22" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" spans="1:5" ht="15" hidden="1">
       <c r="A23" s="8" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="B23" s="9">
-        <v>907.26</v>
+        <v>1014.53</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="10">
@@ -1370,107 +1373,107 @@
         <v>0</v>
       </c>
       <c r="E23" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" hidden="1">
+      <c r="A24" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="9">
+        <v>907.26</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
-      <c r="A24" s="11" t="s">
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+      <c r="A25" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B25" s="9">
         <v>1159.8924999999999</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="11" t="s">
+      <c r="C25" s="8"/>
+      <c r="D25" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" hidden="1">
-      <c r="A25" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="9">
-        <v>2309.7600000000002</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="15" hidden="1">
       <c r="A26" s="8" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="B26" s="9">
-        <v>2710.76</v>
+        <v>2309.7600000000002</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>85</v>
-      </c>
+      <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" ht="15" hidden="1">
       <c r="A27" s="8" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B27" s="9">
-        <v>6397.96</v>
+        <v>2710.76</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" ht="15">
+      <c r="E27" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" hidden="1">
       <c r="A28" s="8" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B28" s="9">
-        <v>5158.8649999999998</v>
-      </c>
-      <c r="C28" s="8">
-        <v>7</v>
-      </c>
+        <v>6397.96</v>
+      </c>
+      <c r="C28" s="8"/>
       <c r="D28" s="10">
         <f t="shared" si="0"/>
-        <v>36112.055</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>85</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" ht="15" hidden="1">
       <c r="A29" s="8" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="B29" s="9">
-        <v>5334.3029999999999</v>
+        <v>5158.8649999999998</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="8"/>
+      <c r="E29" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="15" hidden="1">
       <c r="A30" s="8" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="B30" s="9">
-        <v>5819.5124999999998</v>
+        <v>5334.3029999999999</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="10">
@@ -1481,10 +1484,10 @@
     </row>
     <row r="31" spans="1:5" ht="15" hidden="1">
       <c r="A31" s="8" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="B31" s="9">
-        <v>5607.9849999999997</v>
+        <v>5819.5124999999998</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="10">
@@ -1495,132 +1498,132 @@
     </row>
     <row r="32" spans="1:5" ht="15" hidden="1">
       <c r="A32" s="8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B32" s="9">
-        <v>5793.4475000000002</v>
+        <v>5607.9849999999997</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E32" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="E32" s="8"/>
     </row>
     <row r="33" spans="1:5" ht="15" hidden="1">
       <c r="A33" s="8" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="B33" s="9">
-        <v>7714.2375000000002</v>
+        <v>5793.4475000000002</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E33" s="11"/>
+      <c r="E33" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="15" hidden="1">
       <c r="A34" s="8" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B34" s="9">
-        <v>7722.2574999999997</v>
+        <v>7714.2375000000002</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5" ht="15" hidden="1">
       <c r="A35" s="8" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="B35" s="9">
-        <v>6369.8850000000002</v>
+        <v>7722.2574999999997</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15" hidden="1">
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" ht="15">
       <c r="A36" s="8" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="B36" s="9">
-        <v>8967.36</v>
-      </c>
-      <c r="C36" s="8"/>
+        <v>6369.8850000000002</v>
+      </c>
+      <c r="C36" s="8">
+        <v>20</v>
+      </c>
       <c r="D36" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>127397.70000000001</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" hidden="1">
       <c r="A37" s="8" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B37" s="9">
-        <v>8134.2849999999999</v>
+        <v>8967.36</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E37" s="8"/>
-    </row>
-    <row r="38" spans="1:5" ht="15">
+      <c r="E37" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" hidden="1">
       <c r="A38" s="8" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B38" s="9">
-        <v>1169.9175</v>
-      </c>
-      <c r="C38" s="8">
-        <v>13</v>
-      </c>
+        <v>8134.2849999999999</v>
+      </c>
+      <c r="C38" s="8"/>
       <c r="D38" s="10">
-        <f>C38*B38</f>
-        <v>15208.9275</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E38" s="8"/>
     </row>
     <row r="39" spans="1:5" ht="15" hidden="1">
       <c r="A39" s="8" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B39" s="9">
-        <v>1199.9925000000001</v>
+        <v>1169.9175</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E39" s="8"/>
+        <f>C39*B39</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="15" hidden="1">
       <c r="A40" s="8" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B40" s="9">
-        <v>1189.9675</v>
+        <v>1199.9925000000001</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="10">
@@ -1631,10 +1634,10 @@
     </row>
     <row r="41" spans="1:5" ht="15" hidden="1">
       <c r="A41" s="8" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B41" s="9">
-        <v>1423.55</v>
+        <v>1189.9675</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="10">
@@ -1645,10 +1648,10 @@
     </row>
     <row r="42" spans="1:5" ht="15" hidden="1">
       <c r="A42" s="8" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B42" s="9">
-        <v>1435.58</v>
+        <v>1423.55</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="10">
@@ -1659,111 +1662,111 @@
     </row>
     <row r="43" spans="1:5" ht="15" hidden="1">
       <c r="A43" s="8" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B43" s="9">
-        <v>1053.6275000000001</v>
+        <v>1435.58</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E43" s="8" t="s">
-        <v>87</v>
-      </c>
+      <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5" ht="15" hidden="1">
       <c r="A44" s="8" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B44" s="9">
-        <v>1072.675</v>
+        <v>1053.6275000000001</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E44" s="8"/>
+      <c r="E44" s="8" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="45" spans="1:5" ht="15" hidden="1">
       <c r="A45" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="9">
-        <v>985.46</v>
+        <v>1072.675</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E45" s="8" t="s">
-        <v>102</v>
-      </c>
+      <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" ht="15" hidden="1">
       <c r="A46" s="8" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B46" s="9">
-        <v>1014.53</v>
+        <v>985.46</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E46" s="8"/>
+      <c r="E46" s="8" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="15" hidden="1">
       <c r="A47" s="8" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="B47" s="9">
-        <v>1072.675</v>
+        <v>1014.53</v>
       </c>
       <c r="C47" s="8"/>
-      <c r="D47" s="10"/>
+      <c r="D47" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" ht="15" hidden="1">
       <c r="A48" s="8" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B48" s="9">
-        <v>1077.6875</v>
+        <v>1072.675</v>
       </c>
       <c r="C48" s="8"/>
-      <c r="D48" s="10">
-        <f>B48*C48</f>
-        <v>0</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>86</v>
-      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="8"/>
     </row>
     <row r="49" spans="1:5" ht="15" hidden="1">
       <c r="A49" s="8" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="B49" s="9">
-        <v>1024.5550000000001</v>
+        <v>1077.6875</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E49" s="8"/>
+        <f>B49*C49</f>
+        <v>0</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="50" spans="1:5" ht="15" hidden="1">
       <c r="A50" s="8" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="B50" s="9">
-        <v>1101.7474999999999</v>
+        <v>1024.5550000000001</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="10">
@@ -1774,40 +1777,40 @@
     </row>
     <row r="51" spans="1:5" ht="15" hidden="1">
       <c r="A51" s="8" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B51" s="9">
-        <v>1072.675</v>
+        <v>1101.7474999999999</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E51" s="8" t="s">
-        <v>83</v>
-      </c>
+      <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5" ht="15" hidden="1">
       <c r="A52" s="8" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="B52" s="9">
-        <v>1297.2349999999999</v>
+        <v>1072.675</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E52" s="8"/>
+      <c r="E52" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="53" spans="1:5" ht="15" hidden="1">
       <c r="A53" s="8" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="B53" s="9">
-        <v>11964.8375</v>
+        <v>1297.2349999999999</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="10">
@@ -1818,130 +1821,128 @@
     </row>
     <row r="54" spans="1:5" ht="15" hidden="1">
       <c r="A54" s="8" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="B54" s="9">
-        <v>5607.9849999999997</v>
+        <v>11964.8375</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E54" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="E54" s="8"/>
     </row>
     <row r="55" spans="1:5" ht="15" hidden="1">
       <c r="A55" s="8" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B55" s="9">
-        <v>5183.9274999999998</v>
+        <v>5607.9849999999997</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="10">
-        <f t="shared" ref="D55:D77" si="1">C55*B55</f>
-        <v>0</v>
-      </c>
-      <c r="E55" s="8"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="56" spans="1:5" ht="15" hidden="1">
       <c r="A56" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B56" s="9">
-        <v>5455.6049999999996</v>
+        <v>5183.9274999999998</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D56:D78" si="1">C56*B56</f>
         <v>0</v>
       </c>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="15" hidden="1">
       <c r="A57" s="8" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="B57" s="9">
-        <v>4526.2875000000004</v>
+        <v>5455.6049999999996</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E57" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5" ht="15" hidden="1">
       <c r="A58" s="8" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B58" s="9">
-        <v>5510.7425000000003</v>
+        <v>4526.2875000000004</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E58" s="8"/>
+      <c r="E58" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="59" spans="1:5" ht="15" hidden="1">
       <c r="A59" s="8" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B59" s="9">
-        <v>4896.21</v>
+        <v>5510.7425000000003</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E59" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="E59" s="8"/>
     </row>
     <row r="60" spans="1:5" ht="15" hidden="1">
       <c r="A60" s="8" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B60" s="9">
-        <v>5150.8450000000003</v>
+        <v>4896.21</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E60" s="8"/>
+      <c r="E60" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="15" hidden="1">
       <c r="A61" s="8" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="B61" s="9">
-        <v>4973.4025000000001</v>
+        <v>5150.8450000000003</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E61" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="E61" s="8"/>
     </row>
     <row r="62" spans="1:5" ht="15" hidden="1">
       <c r="A62" s="8" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B62" s="9">
-        <v>4701.7299999999996</v>
+        <v>4973.4025000000001</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="10">
@@ -1949,29 +1950,31 @@
         <v>0</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" hidden="1">
       <c r="A63" s="8" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="B63" s="9">
-        <v>5940.8149999999996</v>
+        <v>4701.7299999999996</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="10">
-        <f>C63*B63</f>
-        <v>0</v>
-      </c>
-      <c r="E63" s="8"/>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="15" hidden="1">
       <c r="A64" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B64" s="9">
-        <v>5257.11</v>
+        <v>5940.8149999999996</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="10">
@@ -1982,40 +1985,38 @@
     </row>
     <row r="65" spans="1:5" ht="15" hidden="1">
       <c r="A65" s="8" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="B65" s="9">
-        <v>3556.87</v>
+        <v>5257.11</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="10">
-        <f t="shared" si="1"/>
+        <f>C65*B65</f>
         <v>0</v>
       </c>
       <c r="E65" s="8"/>
     </row>
     <row r="66" spans="1:5" ht="15" hidden="1">
       <c r="A66" s="8" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B66" s="9">
-        <v>3471.6574999999998</v>
+        <v>3556.87</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E66" s="8" t="s">
-        <v>86</v>
-      </c>
+      <c r="E66" s="8"/>
     </row>
     <row r="67" spans="1:5" ht="15" hidden="1">
       <c r="A67" s="8" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="B67" s="9">
-        <v>3257.1224999999999</v>
+        <v>3471.6574999999998</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="10">
@@ -2023,15 +2024,15 @@
         <v>0</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15" hidden="1">
       <c r="A68" s="8" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B68" s="9">
-        <v>4389.9475000000002</v>
+        <v>3257.1224999999999</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="10">
@@ -2039,15 +2040,15 @@
         <v>0</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15" hidden="1">
       <c r="A69" s="8" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B69" s="9">
-        <v>3618.0225</v>
+        <v>4389.9475000000002</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="10">
@@ -2055,15 +2056,15 @@
         <v>0</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15" hidden="1">
       <c r="A70" s="8" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="B70" s="9">
-        <v>3530.8049999999998</v>
+        <v>3618.0225</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="10">
@@ -2071,29 +2072,31 @@
         <v>0</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" hidden="1">
       <c r="A71" s="8" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B71" s="9">
-        <v>4507.24</v>
+        <v>3530.8049999999998</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E71" s="8"/>
+      <c r="E71" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="72" spans="1:5" ht="15" hidden="1">
       <c r="A72" s="8" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B72" s="9">
-        <v>4408.9949999999999</v>
+        <v>4507.24</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="10">
@@ -2104,26 +2107,24 @@
     </row>
     <row r="73" spans="1:5" ht="15" hidden="1">
       <c r="A73" s="8" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B73" s="9">
-        <v>3979.9250000000002</v>
+        <v>4408.9949999999999</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E73" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="E73" s="8"/>
     </row>
     <row r="74" spans="1:5" ht="15" hidden="1">
       <c r="A74" s="8" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B74" s="9">
-        <v>4115.2624999999998</v>
+        <v>3979.9250000000002</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="10">
@@ -2134,126 +2135,129 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="14.25" hidden="1" customHeight="1">
+    <row r="75" spans="1:5" ht="15" hidden="1">
       <c r="A75" s="8" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B75" s="9">
-        <v>1219.04</v>
+        <v>4115.2624999999998</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="10">
-        <f>B75*C75</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="14.25" customHeight="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="14.25" hidden="1" customHeight="1">
       <c r="A76" s="8" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B76" s="9">
-        <v>1336.3325</v>
-      </c>
-      <c r="C76" s="8">
-        <v>37</v>
-      </c>
+        <v>1219.04</v>
+      </c>
+      <c r="C76" s="8"/>
       <c r="D76" s="10">
         <f>B76*C76</f>
-        <v>49444.302499999998</v>
+        <v>0</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15" hidden="1">
+    <row r="77" spans="1:5" ht="14.25" hidden="1" customHeight="1">
       <c r="A77" s="8" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="B77" s="9">
-        <v>8599.4449999999997</v>
+        <v>1336.3325</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="10">
+        <f>B77*C77</f>
+        <v>0</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15" hidden="1">
+      <c r="A78" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B78" s="9">
+        <v>8599.4449999999997</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E77" s="8"/>
-    </row>
-    <row r="78" spans="1:5" s="2" customFormat="1" ht="15">
-      <c r="A78" s="37" t="s">
+      <c r="E78" s="8"/>
+    </row>
+    <row r="79" spans="1:5" s="2" customFormat="1" ht="15">
+      <c r="A79" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B78" s="37"/>
-      <c r="C78" s="24">
-        <f>SUM(C5:C77)</f>
-        <v>96</v>
-      </c>
-      <c r="D78" s="25">
-        <f>SUM(D5:D77)</f>
-        <v>134232.745</v>
-      </c>
-      <c r="E78" s="24"/>
-    </row>
-    <row r="79" spans="1:5" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A79" s="3"/>
-    </row>
-    <row r="80" spans="1:5" s="22" customFormat="1" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A80" s="39"/>
-      <c r="B80" s="40"/>
-      <c r="C80" s="40"/>
-      <c r="D80" s="41"/>
-      <c r="E80" s="21"/>
-    </row>
-    <row r="81" spans="1:9" s="22" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A81" s="23"/>
-      <c r="B81" s="23"/>
-      <c r="C81" s="23"/>
-      <c r="D81" s="23"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="24">
+        <f>SUM(C5:C78)</f>
+        <v>116</v>
+      </c>
+      <c r="D79" s="25">
+        <f>SUM(D5:D78)</f>
+        <v>218545.29</v>
+      </c>
+      <c r="E79" s="24"/>
+    </row>
+    <row r="80" spans="1:5" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A80" s="3"/>
+    </row>
+    <row r="81" spans="1:9" s="22" customFormat="1" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A81" s="39"/>
+      <c r="B81" s="40"/>
+      <c r="C81" s="40"/>
+      <c r="D81" s="41"/>
       <c r="E81" s="21"/>
     </row>
-    <row r="82" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A82" s="13"/>
-      <c r="B82" s="38" t="s">
+    <row r="82" spans="1:9" s="22" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A82" s="23"/>
+      <c r="B82" s="23"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="21"/>
+    </row>
+    <row r="83" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A83" s="13"/>
+      <c r="B83" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C82" s="38"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="14"/>
-    </row>
-    <row r="83" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A83" s="15"/>
-      <c r="B83" s="16" t="s">
+      <c r="C83" s="38"/>
+      <c r="D83" s="38"/>
+      <c r="E83" s="14"/>
+    </row>
+    <row r="84" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A84" s="15"/>
+      <c r="B84" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C83" s="16" t="s">
+      <c r="C84" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D83" s="16" t="s">
+      <c r="D84" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E83" s="14"/>
-      <c r="I83" s="17"/>
-    </row>
-    <row r="84" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A84" s="18"/>
-      <c r="B84" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C84" s="29"/>
-      <c r="D84" s="8"/>
       <c r="E84" s="14"/>
+      <c r="I84" s="17"/>
     </row>
     <row r="85" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A85" s="18"/>
       <c r="B85" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C85" s="29">
-        <v>140000</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C85" s="29"/>
       <c r="D85" s="8"/>
       <c r="E85" s="14"/>
     </row>
@@ -2262,14 +2266,16 @@
       <c r="B86" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C86" s="29"/>
+      <c r="C86" s="29">
+        <v>220000</v>
+      </c>
       <c r="D86" s="8"/>
       <c r="E86" s="14"/>
     </row>
     <row r="87" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A87" s="18"/>
       <c r="B87" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C87" s="29"/>
       <c r="D87" s="8"/>
@@ -2278,7 +2284,7 @@
     <row r="88" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A88" s="18"/>
       <c r="B88" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C88" s="29"/>
       <c r="D88" s="8"/>
@@ -2287,31 +2293,40 @@
     <row r="89" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A89" s="18"/>
       <c r="B89" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C89" s="29"/>
       <c r="D89" s="8"/>
       <c r="E89" s="14"/>
     </row>
     <row r="90" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A90" s="15"/>
-      <c r="B90" s="19" t="s">
+      <c r="A90" s="18"/>
+      <c r="B90" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C90" s="29"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="14"/>
+    </row>
+    <row r="91" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A91" s="15"/>
+      <c r="B91" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C90" s="30">
-        <f>SUM(C84:C89)</f>
-        <v>140000</v>
-      </c>
-      <c r="D90" s="20"/>
-      <c r="E90" s="14"/>
-    </row>
-    <row r="91" spans="1:9">
-      <c r="A91" s="3"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
+      <c r="C91" s="30">
+        <f>SUM(C85:C90)</f>
+        <v>220000</v>
+      </c>
+      <c r="D91" s="20"/>
+      <c r="E91" s="14"/>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" s="3"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:E78">
+  <autoFilter ref="A4:E79">
     <filterColumn colId="2">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -2321,9 +2336,9 @@
   <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="A81:D81"/>
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2335,8 +2350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection sqref="A1:E43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
23.07.19 Today & 24.07.19 Apple+Ratri Hisab Updated
</commit_message>
<xml_diff>
--- a/July/Others/Requisition of Tulip-2/Requisition of Tulip-2.xlsx
+++ b/July/Others/Requisition of Tulip-2/Requisition of Tulip-2.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Daily Requisition" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Daily Requisition'!$A$4:$E$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Daily Requisition'!$A$4:$E$80</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="107">
   <si>
     <t>Model Name</t>
   </si>
@@ -337,9 +337,6 @@
     <t>BL97</t>
   </si>
   <si>
-    <t>Gold/Black</t>
-  </si>
-  <si>
     <r>
       <t>Black/</t>
     </r>
@@ -358,9 +355,6 @@
     <t>Dealer Name:   Tulip-2</t>
   </si>
   <si>
-    <t>22.07.19</t>
-  </si>
-  <si>
     <r>
       <t>Black/</t>
     </r>
@@ -374,6 +368,12 @@
       </rPr>
       <t xml:space="preserve"> Not_Red</t>
     </r>
+  </si>
+  <si>
+    <t>B65</t>
+  </si>
+  <si>
+    <t>23.07.19</t>
   </si>
 </sst>
 </file>
@@ -571,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -606,7 +606,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -647,7 +646,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -996,13 +994,13 @@
   <sheetPr filterMode="1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F91" sqref="F91"/>
+      <selection pane="bottomRight" activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1016,34 +1014,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="12.75">
-      <c r="A1" s="37"/>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="39"/>
+      <c r="A1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5" s="6" customFormat="1" ht="15.75">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="42"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15">
-      <c r="A3" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="21" t="s">
+      <c r="A3" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="45"/>
+      <c r="C3" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="23" t="s">
-        <v>105</v>
+      <c r="E3" s="22" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="6" customFormat="1" ht="12.75">
@@ -1088,7 +1086,7 @@
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="10">
-        <f t="shared" ref="D6:D55" si="0">C6*B6</f>
+        <f t="shared" ref="D6:D56" si="0">C6*B6</f>
         <v>0</v>
       </c>
       <c r="E6" s="8"/>
@@ -1107,22 +1105,20 @@
       </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" ht="15" hidden="1">
       <c r="A8" s="8" t="s">
         <v>91</v>
       </c>
       <c r="B8" s="9">
         <v>760.9</v>
       </c>
-      <c r="C8" s="8">
-        <v>80</v>
-      </c>
+      <c r="C8" s="8"/>
       <c r="D8" s="10">
         <f>C8*B8</f>
-        <v>60872</v>
+        <v>0</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" hidden="1">
@@ -1157,58 +1153,60 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:5" ht="15">
+      <c r="A11" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="9">
+        <v>770.92</v>
+      </c>
+      <c r="C11" s="8">
+        <v>150</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" si="0"/>
+        <v>115638</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+      <c r="A12" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B12" s="9">
         <v>896.23500000000001</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="11" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" hidden="1">
-      <c r="A12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="9">
-        <v>868.16499999999996</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" ht="15" hidden="1">
       <c r="A13" s="8" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B13" s="9">
-        <v>901.24749999999995</v>
+        <v>868.16499999999996</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>82</v>
-      </c>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" ht="15" hidden="1">
       <c r="A14" s="8" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="B14" s="9">
-        <v>858.14</v>
+        <v>901.24749999999995</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="10">
@@ -1216,155 +1214,153 @@
         <v>0</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" hidden="1">
       <c r="A15" s="8" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="B15" s="9">
-        <v>824.06</v>
+        <v>858.14</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="10">
-        <f>B15*C15</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
-      <c r="A16" s="11" t="s">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" hidden="1">
+      <c r="A16" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="9">
+        <v>824.06</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="10">
+        <f>B16*C16</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+      <c r="A17" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B17" s="9">
         <v>858.14</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="11" t="s">
+      <c r="C17" s="8"/>
+      <c r="D17" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" hidden="1">
-      <c r="A17" s="8" t="s">
+    <row r="18" spans="1:5" ht="15" hidden="1">
+      <c r="A18" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B18" s="9">
         <v>946.36</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
-      <c r="A18" s="11" t="s">
+      <c r="C18" s="8"/>
+      <c r="D18" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+      <c r="A19" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B19" s="9">
         <v>980.44500000000005</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="12">
-        <f>C18*B18</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="11" t="s">
+      <c r="C19" s="8"/>
+      <c r="D19" s="12">
+        <f>C19*B19</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" hidden="1">
-      <c r="A19" s="8" t="s">
+    <row r="20" spans="1:5" ht="15" hidden="1">
+      <c r="A20" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B20" s="9">
         <v>975.4325</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="8" t="s">
+      <c r="C20" s="8"/>
+      <c r="D20" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15">
-      <c r="A20" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="9">
-        <v>1159.8900000000001</v>
-      </c>
-      <c r="C20" s="8">
-        <v>40</v>
-      </c>
-      <c r="D20" s="10">
-        <f>B20*C20</f>
-        <v>46395.600000000006</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" hidden="1">
       <c r="A21" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="9">
+        <v>1159.8900000000001</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="10">
+        <f>B21*C21</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" hidden="1">
+      <c r="A22" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B22" s="9">
         <v>1140.845</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="12">
-        <f>C21*B21</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
-      <c r="A22" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="9">
-        <v>936.34</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="1:5" ht="15" hidden="1">
-      <c r="A23" s="8" t="s">
-        <v>59</v>
+        <f>C22*B22</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+      <c r="A23" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="B23" s="9">
-        <v>1014.53</v>
+        <v>936.34</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>84</v>
-      </c>
+      <c r="D23" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:5" ht="15" hidden="1">
       <c r="A24" s="8" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="B24" s="9">
-        <v>907.26</v>
+        <v>1014.53</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="10">
@@ -1372,105 +1368,107 @@
         <v>0</v>
       </c>
       <c r="E24" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" hidden="1">
+      <c r="A25" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="9">
+        <v>907.26</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
-      <c r="A25" s="11" t="s">
+    <row r="26" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+      <c r="A26" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B26" s="9">
         <v>1159.8924999999999</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="11" t="s">
+      <c r="C26" s="8"/>
+      <c r="D26" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" hidden="1">
-      <c r="A26" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="9">
-        <v>2309.7600000000002</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" ht="15" hidden="1">
       <c r="A27" s="8" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="B27" s="9">
-        <v>2710.76</v>
+        <v>2309.7600000000002</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="11" t="s">
-        <v>84</v>
-      </c>
+      <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" ht="15" hidden="1">
       <c r="A28" s="8" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B28" s="9">
-        <v>6397.96</v>
+        <v>2710.76</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E28" s="8"/>
+      <c r="E28" s="11" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="15" hidden="1">
       <c r="A29" s="8" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B29" s="9">
-        <v>5158.8649999999998</v>
+        <v>6397.96</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>84</v>
-      </c>
+      <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" ht="15" hidden="1">
       <c r="A30" s="8" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="B30" s="9">
-        <v>5334.3029999999999</v>
+        <v>5158.8649999999998</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E30" s="8"/>
+      <c r="E30" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="15" hidden="1">
       <c r="A31" s="8" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="B31" s="9">
-        <v>5819.5124999999998</v>
+        <v>5334.3029999999999</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="10">
@@ -1481,10 +1479,10 @@
     </row>
     <row r="32" spans="1:5" ht="15" hidden="1">
       <c r="A32" s="8" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="B32" s="9">
-        <v>5607.9849999999997</v>
+        <v>5819.5124999999998</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="10">
@@ -1495,130 +1493,134 @@
     </row>
     <row r="33" spans="1:5" ht="15" hidden="1">
       <c r="A33" s="8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B33" s="9">
-        <v>5793.4475000000002</v>
+        <v>5607.9849999999997</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E33" s="8" t="s">
-        <v>84</v>
-      </c>
+      <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5" ht="15" hidden="1">
       <c r="A34" s="8" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="B34" s="9">
-        <v>7714.2375000000002</v>
+        <v>5793.4475000000002</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="11"/>
+      <c r="E34" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="15" hidden="1">
       <c r="A35" s="8" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B35" s="9">
-        <v>7722.2574999999997</v>
+        <v>7714.2375000000002</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="8"/>
+      <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:5" ht="15" hidden="1">
       <c r="A36" s="8" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="B36" s="9">
-        <v>6369.8850000000002</v>
+        <v>7722.2574999999997</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" hidden="1">
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" ht="15">
       <c r="A37" s="8" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="B37" s="9">
-        <v>8967.36</v>
-      </c>
-      <c r="C37" s="8"/>
+        <v>6369.8850000000002</v>
+      </c>
+      <c r="C37" s="8">
+        <v>5</v>
+      </c>
       <c r="D37" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31849.425000000003</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" hidden="1">
+    <row r="38" spans="1:5" ht="15">
       <c r="A38" s="8" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B38" s="9">
-        <v>8134.2849999999999</v>
-      </c>
-      <c r="C38" s="8"/>
+        <v>8967.36</v>
+      </c>
+      <c r="C38" s="8">
+        <v>2</v>
+      </c>
       <c r="D38" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E38" s="8"/>
+        <v>17934.72</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="15" hidden="1">
       <c r="A39" s="8" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B39" s="9">
-        <v>1169.9175</v>
+        <v>8134.2849999999999</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="10">
-        <f>C39*B39</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>96</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" ht="15" hidden="1">
       <c r="A40" s="8" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B40" s="9">
-        <v>1199.9925000000001</v>
+        <v>1169.9175</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="8"/>
+        <f>C40*B40</f>
+        <v>0</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="41" spans="1:5" ht="15" hidden="1">
       <c r="A41" s="8" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B41" s="9">
-        <v>1189.9675</v>
+        <v>1199.9925000000001</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="10">
@@ -1629,10 +1631,10 @@
     </row>
     <row r="42" spans="1:5" ht="15" hidden="1">
       <c r="A42" s="8" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B42" s="9">
-        <v>1423.55</v>
+        <v>1189.9675</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="10">
@@ -1643,10 +1645,10 @@
     </row>
     <row r="43" spans="1:5" ht="15" hidden="1">
       <c r="A43" s="8" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B43" s="9">
-        <v>1435.58</v>
+        <v>1423.55</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="10">
@@ -1657,159 +1659,157 @@
     </row>
     <row r="44" spans="1:5" ht="15" hidden="1">
       <c r="A44" s="8" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B44" s="9">
-        <v>1053.6275000000001</v>
+        <v>1435.58</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E44" s="8" t="s">
-        <v>86</v>
-      </c>
+      <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5" ht="15" hidden="1">
       <c r="A45" s="8" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B45" s="9">
-        <v>1072.675</v>
+        <v>1053.6275000000001</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E45" s="8"/>
-    </row>
-    <row r="46" spans="1:5" ht="15">
+      <c r="E45" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" hidden="1">
       <c r="A46" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="9">
-        <v>985.46</v>
-      </c>
-      <c r="C46" s="8">
-        <v>100</v>
-      </c>
+        <v>1072.675</v>
+      </c>
+      <c r="C46" s="8"/>
       <c r="D46" s="10">
         <f t="shared" si="0"/>
-        <v>98546</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>106</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E46" s="8"/>
     </row>
     <row r="47" spans="1:5" ht="15" hidden="1">
       <c r="A47" s="8" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B47" s="9">
-        <v>1014.53</v>
+        <v>985.46</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E47" s="8"/>
+      <c r="E47" s="8" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="15" hidden="1">
       <c r="A48" s="8" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="B48" s="9">
-        <v>1072.675</v>
+        <v>1014.53</v>
       </c>
       <c r="C48" s="8"/>
-      <c r="D48" s="10"/>
+      <c r="D48" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E48" s="8"/>
     </row>
     <row r="49" spans="1:5" ht="15" hidden="1">
       <c r="A49" s="8" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B49" s="9">
-        <v>1077.6875</v>
+        <v>1072.675</v>
       </c>
       <c r="C49" s="8"/>
-      <c r="D49" s="10">
-        <f>B49*C49</f>
-        <v>0</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="D49" s="10"/>
+      <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" ht="15" hidden="1">
       <c r="A50" s="8" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="B50" s="9">
-        <v>1024.5550000000001</v>
+        <v>1077.6875</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="10">
-        <f t="shared" si="0"/>
+        <f>B50*C50</f>
         <v>0</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" hidden="1">
       <c r="A51" s="8" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="B51" s="9">
-        <v>1101.7474999999999</v>
+        <v>1024.5550000000001</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E51" s="8"/>
+      <c r="E51" s="8" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="52" spans="1:5" ht="15" hidden="1">
       <c r="A52" s="8" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B52" s="9">
-        <v>1072.675</v>
+        <v>1101.7474999999999</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E52" s="8" t="s">
-        <v>82</v>
-      </c>
+      <c r="E52" s="8"/>
     </row>
     <row r="53" spans="1:5" ht="15" hidden="1">
       <c r="A53" s="8" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="B53" s="9">
-        <v>1297.2349999999999</v>
+        <v>1072.675</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E53" s="8"/>
+      <c r="E53" s="8" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="15" hidden="1">
       <c r="A54" s="8" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="B54" s="9">
-        <v>11964.8375</v>
+        <v>1297.2349999999999</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="10">
@@ -1820,130 +1820,128 @@
     </row>
     <row r="55" spans="1:5" ht="15" hidden="1">
       <c r="A55" s="8" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="B55" s="9">
-        <v>5607.9849999999997</v>
+        <v>11964.8375</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E55" s="8" t="s">
-        <v>84</v>
-      </c>
+      <c r="E55" s="8"/>
     </row>
     <row r="56" spans="1:5" ht="15" hidden="1">
       <c r="A56" s="8" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B56" s="9">
-        <v>5183.9274999999998</v>
+        <v>5607.9849999999997</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="10">
-        <f t="shared" ref="D56:D78" si="1">C56*B56</f>
-        <v>0</v>
-      </c>
-      <c r="E56" s="8"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="57" spans="1:5" ht="15" hidden="1">
       <c r="A57" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B57" s="9">
-        <v>5455.6049999999996</v>
+        <v>5183.9274999999998</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D57:D79" si="1">C57*B57</f>
         <v>0</v>
       </c>
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5" ht="15" hidden="1">
       <c r="A58" s="8" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="B58" s="9">
-        <v>4526.2875000000004</v>
+        <v>5455.6049999999996</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E58" s="8" t="s">
-        <v>84</v>
-      </c>
+      <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5" ht="15" hidden="1">
       <c r="A59" s="8" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B59" s="9">
-        <v>5510.7425000000003</v>
+        <v>4526.2875000000004</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E59" s="8"/>
+      <c r="E59" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="60" spans="1:5" ht="15" hidden="1">
       <c r="A60" s="8" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B60" s="9">
-        <v>4896.21</v>
+        <v>5510.7425000000003</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E60" s="8" t="s">
-        <v>84</v>
-      </c>
+      <c r="E60" s="8"/>
     </row>
     <row r="61" spans="1:5" ht="15" hidden="1">
       <c r="A61" s="8" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B61" s="9">
-        <v>5150.8450000000003</v>
+        <v>4896.21</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E61" s="8"/>
+      <c r="E61" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="15" hidden="1">
       <c r="A62" s="8" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="B62" s="9">
-        <v>4973.4025000000001</v>
+        <v>5150.8450000000003</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E62" s="8" t="s">
-        <v>84</v>
-      </c>
+      <c r="E62" s="8"/>
     </row>
     <row r="63" spans="1:5" ht="15" hidden="1">
       <c r="A63" s="8" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B63" s="9">
-        <v>4701.7299999999996</v>
+        <v>4973.4025000000001</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="10">
@@ -1951,29 +1949,31 @@
         <v>0</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15" hidden="1">
       <c r="A64" s="8" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="B64" s="9">
-        <v>5940.8149999999996</v>
+        <v>4701.7299999999996</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="10">
-        <f>C64*B64</f>
-        <v>0</v>
-      </c>
-      <c r="E64" s="8"/>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="65" spans="1:5" ht="15" hidden="1">
       <c r="A65" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B65" s="9">
-        <v>5257.11</v>
+        <v>5940.8149999999996</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="10">
@@ -1984,40 +1984,38 @@
     </row>
     <row r="66" spans="1:5" ht="15" hidden="1">
       <c r="A66" s="8" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="B66" s="9">
-        <v>3556.87</v>
+        <v>5257.11</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="10">
-        <f t="shared" si="1"/>
+        <f>C66*B66</f>
         <v>0</v>
       </c>
       <c r="E66" s="8"/>
     </row>
     <row r="67" spans="1:5" ht="15" hidden="1">
       <c r="A67" s="8" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B67" s="9">
-        <v>3471.6574999999998</v>
+        <v>3556.87</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E67" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="E67" s="8"/>
     </row>
     <row r="68" spans="1:5" ht="15" hidden="1">
       <c r="A68" s="8" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="B68" s="9">
-        <v>3257.1224999999999</v>
+        <v>3471.6574999999998</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="10">
@@ -2025,15 +2023,15 @@
         <v>0</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15" hidden="1">
       <c r="A69" s="8" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B69" s="9">
-        <v>4389.9475000000002</v>
+        <v>3257.1224999999999</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="10">
@@ -2041,15 +2039,15 @@
         <v>0</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15" hidden="1">
       <c r="A70" s="8" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B70" s="9">
-        <v>3618.0225</v>
+        <v>4389.9475000000002</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="10">
@@ -2057,15 +2055,15 @@
         <v>0</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" hidden="1">
       <c r="A71" s="8" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="B71" s="9">
-        <v>3530.8049999999998</v>
+        <v>3618.0225</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="10">
@@ -2073,29 +2071,31 @@
         <v>0</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15" hidden="1">
       <c r="A72" s="8" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B72" s="9">
-        <v>4507.24</v>
+        <v>3530.8049999999998</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E72" s="8"/>
+      <c r="E72" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="73" spans="1:5" ht="15" hidden="1">
       <c r="A73" s="8" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B73" s="9">
-        <v>4408.9949999999999</v>
+        <v>4507.24</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="10">
@@ -2106,26 +2106,24 @@
     </row>
     <row r="74" spans="1:5" ht="15" hidden="1">
       <c r="A74" s="8" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B74" s="9">
-        <v>3979.9250000000002</v>
+        <v>4408.9949999999999</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E74" s="8" t="s">
-        <v>84</v>
-      </c>
+      <c r="E74" s="8"/>
     </row>
     <row r="75" spans="1:5" ht="15" hidden="1">
       <c r="A75" s="8" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B75" s="9">
-        <v>4115.2624999999998</v>
+        <v>3979.9250000000002</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="10">
@@ -2136,28 +2134,28 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="14.25" hidden="1" customHeight="1">
+    <row r="76" spans="1:5" ht="15" hidden="1">
       <c r="A76" s="8" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="B76" s="9">
-        <v>1219.04</v>
+        <v>4115.2624999999998</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="10">
-        <f>B76*C76</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="14.25" hidden="1" customHeight="1">
       <c r="A77" s="8" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B77" s="9">
-        <v>1336.3325</v>
+        <v>1219.04</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="10">
@@ -2168,165 +2166,184 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15" hidden="1">
+    <row r="78" spans="1:5" ht="14.25" hidden="1" customHeight="1">
       <c r="A78" s="8" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="B78" s="9">
-        <v>8599.4449999999997</v>
+        <v>1336.3325</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="10">
+        <f>B78*C78</f>
+        <v>0</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15" hidden="1">
+      <c r="A79" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B79" s="9">
+        <v>8599.4449999999997</v>
+      </c>
+      <c r="C79" s="8"/>
+      <c r="D79" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E78" s="8"/>
-    </row>
-    <row r="79" spans="1:5" s="2" customFormat="1" ht="15">
-      <c r="A79" s="43" t="s">
+      <c r="E79" s="8"/>
+    </row>
+    <row r="80" spans="1:5" s="2" customFormat="1" ht="15">
+      <c r="A80" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B79" s="43"/>
-      <c r="C79" s="19">
-        <f>SUM(C5:C78)</f>
-        <v>220</v>
-      </c>
-      <c r="D79" s="20">
-        <f>SUM(D5:D78)</f>
-        <v>205813.6</v>
-      </c>
-      <c r="E79" s="19"/>
-    </row>
-    <row r="80" spans="1:5" ht="17.25" customHeight="1">
-      <c r="A80" s="3"/>
-    </row>
-    <row r="81" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A81" s="45"/>
-      <c r="B81" s="45"/>
-      <c r="C81" s="45"/>
-      <c r="D81" s="45"/>
-      <c r="E81" s="26"/>
-    </row>
-    <row r="82" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A82" s="32"/>
-      <c r="B82" s="18"/>
-      <c r="C82" s="18"/>
-      <c r="D82" s="18"/>
-      <c r="E82" s="26"/>
-      <c r="F82" s="29"/>
-    </row>
-    <row r="83" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A83" s="33"/>
-      <c r="B83" s="44" t="s">
+      <c r="B80" s="41"/>
+      <c r="C80" s="18">
+        <f>SUM(C5:C79)</f>
+        <v>157</v>
+      </c>
+      <c r="D80" s="19">
+        <f>SUM(D5:D79)</f>
+        <v>165422.14499999999</v>
+      </c>
+      <c r="E80" s="18"/>
+    </row>
+    <row r="81" spans="1:9" ht="17.25" customHeight="1">
+      <c r="A81" s="3"/>
+    </row>
+    <row r="82" spans="1:9" s="16" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A82" s="43"/>
+      <c r="B82" s="43"/>
+      <c r="C82" s="43"/>
+      <c r="D82" s="43"/>
+      <c r="E82" s="25"/>
+    </row>
+    <row r="83" spans="1:9" s="16" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A83" s="30"/>
+      <c r="B83" s="17"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="25"/>
+    </row>
+    <row r="84" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A84" s="31"/>
+      <c r="B84" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C83" s="44"/>
-      <c r="D83" s="44"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="30"/>
-    </row>
-    <row r="84" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A84" s="34"/>
-      <c r="B84" s="13" t="s">
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="26"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="16"/>
+    </row>
+    <row r="85" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A85" s="32"/>
+      <c r="B85" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C84" s="13" t="s">
+      <c r="C85" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D84" s="13" t="s">
+      <c r="D85" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E84" s="27"/>
-      <c r="F84" s="30"/>
-      <c r="I84" s="14"/>
-    </row>
-    <row r="85" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A85" s="35"/>
-      <c r="B85" s="8" t="s">
+      <c r="E85" s="26"/>
+      <c r="F85" s="28"/>
+    </row>
+    <row r="86" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A86" s="33"/>
+      <c r="B86" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C85" s="24"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="27"/>
-      <c r="F85" s="30"/>
-    </row>
-    <row r="86" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A86" s="35"/>
-      <c r="B86" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C86" s="24">
-        <v>220000</v>
-      </c>
+      <c r="C86" s="23"/>
       <c r="D86" s="8"/>
-      <c r="E86" s="27"/>
-      <c r="F86" s="30"/>
+      <c r="E86" s="26"/>
     </row>
     <row r="87" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A87" s="35"/>
+      <c r="A87" s="33"/>
       <c r="B87" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C87" s="24"/>
+      <c r="C87" s="23">
+        <v>200000</v>
+      </c>
       <c r="D87" s="8"/>
-      <c r="E87" s="27"/>
-      <c r="F87" s="30"/>
+      <c r="E87" s="26"/>
+      <c r="F87" s="28"/>
+      <c r="G87" s="28"/>
+      <c r="H87" s="28"/>
+      <c r="I87" s="28"/>
     </row>
     <row r="88" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A88" s="35"/>
+      <c r="A88" s="33"/>
       <c r="B88" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" s="23"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="26"/>
+      <c r="F88" s="28"/>
+      <c r="G88" s="28"/>
+      <c r="H88" s="28"/>
+      <c r="I88" s="28"/>
+    </row>
+    <row r="89" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A89" s="33"/>
+      <c r="B89" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C88" s="24"/>
-      <c r="D88" s="8"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="30"/>
-    </row>
-    <row r="89" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A89" s="35"/>
-      <c r="B89" s="8" t="s">
+      <c r="C89" s="23"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="26"/>
+      <c r="F89" s="28"/>
+    </row>
+    <row r="90" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A90" s="33"/>
+      <c r="B90" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C89" s="24"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="30"/>
-    </row>
-    <row r="90" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A90" s="35"/>
-      <c r="B90" s="8" t="s">
+      <c r="C90" s="23"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="26"/>
+      <c r="F90" s="28"/>
+    </row>
+    <row r="91" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A91" s="33"/>
+      <c r="B91" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C90" s="24"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="27"/>
-      <c r="F90" s="30"/>
-    </row>
-    <row r="91" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A91" s="34"/>
-      <c r="B91" s="15" t="s">
+      <c r="C91" s="23"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="26"/>
+      <c r="F91" s="28"/>
+    </row>
+    <row r="92" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A92" s="32"/>
+      <c r="B92" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C91" s="25">
-        <f>SUM(C85:C90)</f>
-        <v>220000</v>
-      </c>
-      <c r="D91" s="16"/>
-      <c r="E91" s="27"/>
-      <c r="F91" s="30"/>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="A92" s="36"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="28"/>
-      <c r="F92" s="31"/>
+      <c r="C92" s="24">
+        <v>200000</v>
+      </c>
+      <c r="D92" s="15"/>
+      <c r="E92" s="26"/>
+      <c r="F92" s="28"/>
     </row>
     <row r="93" spans="1:9">
-      <c r="E93" s="28"/>
+      <c r="A93" s="34"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="27"/>
+      <c r="F93" s="29"/>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="E94" s="27"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:E79">
+  <autoFilter ref="A4:E80">
     <filterColumn colId="2">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -2336,9 +2353,9 @@
   <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="A82:D82"/>
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>